<commit_message>
Completed implementation of no student id
The application can now be fully used with empty student IDs.

The students who don't have IDs are given an ID that is randomly
generated at their import time (with a special prefix so that you know
that it's been randomly generated) and works this way.

Therefore, #69 has been resolved.
</commit_message>
<xml_diff>
--- a/test/Test Sheet.xlsx
+++ b/test/Test Sheet.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9555" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9560" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Grade 9" sheetId="1" r:id="rId1"/>
     <sheet name="Grade 10" sheetId="2" r:id="rId2"/>
     <sheet name="Grade 11" sheetId="3" r:id="rId3"/>
     <sheet name="Grade 12" sheetId="4" r:id="rId4"/>
+    <sheet name="TestNoStudentIDs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="163">
   <si>
     <t>First</t>
   </si>
@@ -504,6 +505,18 @@
   </si>
   <si>
     <t>Last 12-19</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Student ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grade </t>
   </si>
 </sst>
 </file>
@@ -824,12 +837,12 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E21"/>
+      <selection activeCell="A6" sqref="A6:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -863,7 +876,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -880,7 +893,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -897,7 +910,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -914,7 +927,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -931,7 +944,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -948,7 +961,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -965,7 +978,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -982,7 +995,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -999,7 +1012,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1016,7 +1029,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +1046,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1050,7 +1063,7 @@
         <v>903</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1067,7 +1080,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1084,7 +1097,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1101,7 +1114,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1118,7 +1131,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1135,7 +1148,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1152,7 +1165,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1169,7 +1182,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1196,12 +1209,12 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1235,7 +1248,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1252,7 +1265,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1269,7 +1282,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -1286,7 +1299,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -1303,7 +1316,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -1320,7 +1333,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1337,7 +1350,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1354,7 +1367,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1371,7 +1384,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -1388,7 +1401,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1405,7 +1418,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1422,7 +1435,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -1439,7 +1452,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>69</v>
       </c>
@@ -1456,7 +1469,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1473,7 +1486,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>73</v>
       </c>
@@ -1490,7 +1503,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>75</v>
       </c>
@@ -1507,7 +1520,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -1524,7 +1537,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>118</v>
       </c>
@@ -1541,7 +1554,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1568,12 +1581,12 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A14" sqref="A14:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1590,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -1607,7 +1620,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -1624,7 +1637,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1641,7 +1654,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>87</v>
       </c>
@@ -1658,7 +1671,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1675,7 +1688,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -1692,7 +1705,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -1709,7 +1722,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -1726,7 +1739,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>97</v>
       </c>
@@ -1743,7 +1756,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -1760,7 +1773,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>97</v>
       </c>
@@ -1777,7 +1790,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -1794,7 +1807,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -1811,7 +1824,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1828,7 +1841,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -1845,7 +1858,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>109</v>
       </c>
@@ -1862,7 +1875,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>111</v>
       </c>
@@ -1879,7 +1892,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>113</v>
       </c>
@@ -1896,7 +1909,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -1913,7 +1926,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>115</v>
       </c>
@@ -1939,13 +1952,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1979,7 +1992,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>123</v>
       </c>
@@ -1996,7 +2009,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>125</v>
       </c>
@@ -2013,7 +2026,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>127</v>
       </c>
@@ -2030,7 +2043,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>129</v>
       </c>
@@ -2047,7 +2060,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>131</v>
       </c>
@@ -2064,7 +2077,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -2081,7 +2094,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -2098,7 +2111,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>137</v>
       </c>
@@ -2115,7 +2128,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>139</v>
       </c>
@@ -2132,7 +2145,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -2149,7 +2162,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -2166,7 +2179,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -2183,7 +2196,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>145</v>
       </c>
@@ -2200,7 +2213,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>147</v>
       </c>
@@ -2217,7 +2230,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -2234,7 +2247,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -2251,7 +2264,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -2268,7 +2281,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>157</v>
       </c>
@@ -2285,7 +2298,7 @@
         <v>1205</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -2300,6 +2313,262 @@
       </c>
       <c r="E21">
         <v>1205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17">
+        <v>1104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>